<commit_message>
fix: Edad de 115
</commit_message>
<xml_diff>
--- a/Resultados/data/invalidez.xlsx
+++ b/Resultados/data/invalidez.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f07da985e540e617/Documents/Universidad/7 - Séptimo semestre/Pensiones I/Proyecto_pensiones_I/Resultados/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{447A53CD-3957-4504-9EDD-1056EAE0E778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{447A53CD-3957-4504-9EDD-1056EAE0E778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB78D870-D6A9-45BF-94AE-FED5C03A34CC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7B3194A1-872D-4828-803D-D33652AD1ED5}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja 1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$C$97</definedName>
+    <definedName name="DatosExternos_1" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$C$98</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -485,8 +485,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB0BDCF5-958B-40F1-9BC7-A273677BE97C}" name="Table007__Page_5" displayName="Table007__Page_5" ref="A1:C97" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C97" xr:uid="{DB0BDCF5-958B-40F1-9BC7-A273677BE97C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB0BDCF5-958B-40F1-9BC7-A273677BE97C}" name="Table007__Page_5" displayName="Table007__Page_5" ref="A1:C98" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C98" xr:uid="{DB0BDCF5-958B-40F1-9BC7-A273677BE97C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BAE26F04-9674-4C66-A50A-7CFB1C40068A}" uniqueName="1" name="Edad" queryTableFieldId="1" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{839CFA1F-F537-4460-B6AC-54A31CFD55C7}" uniqueName="2" name="Hombres" queryTableFieldId="2" dataDxfId="1"/>
@@ -813,1079 +813,1090 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BD9DC8-8404-489F-9DA2-D872A632889E}">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>78</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>84</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>86</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
         <v>95</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>96</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="A31" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>99</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="A32" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>102</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="A33" t="s">
         <v>104</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>105</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" t="s">
         <v>107</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>108</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="A35" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" t="s">
         <v>111</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37">
         <v>54</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>3</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38">
         <v>55</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39">
         <v>56</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="A40">
         <v>57</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41">
         <v>58</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42">
         <v>59</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>24</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43">
         <v>60</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="A44">
         <v>61</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="A45">
         <v>62</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="A46">
         <v>63</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>64</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="A47">
+        <v>64</v>
+      </c>
+      <c r="B47" t="s">
         <v>43</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="A48">
         <v>65</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49">
         <v>66</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="A50">
         <v>67</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="A51">
         <v>68</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+      <c r="A52">
         <v>69</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+      <c r="A53">
         <v>70</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="B53" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+      <c r="A54">
         <v>71</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C54" s="1" t="s">
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="A55">
         <v>72</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C55" s="1" t="s">
+      <c r="B55" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="A56">
         <v>73</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C56" s="1" t="s">
+      <c r="B56" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="A57">
         <v>74</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="B57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="A58">
         <v>75</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" s="1" t="s">
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="A59">
         <v>76</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+      <c r="A60">
         <v>77</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C60" s="1" t="s">
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="A61">
         <v>78</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="1" t="s">
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+      <c r="A62">
         <v>79</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+      <c r="A63">
         <v>80</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C63" s="1" t="s">
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+      <c r="A64">
         <v>81</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C64" s="1" t="s">
+      <c r="B64" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+      <c r="A65">
         <v>82</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C65" s="1" t="s">
+      <c r="B65" t="s">
+        <v>64</v>
+      </c>
+      <c r="C65" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+      <c r="A66">
         <v>83</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C66" s="1" t="s">
+      <c r="B66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+      <c r="A67">
         <v>84</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C67" s="1" t="s">
+      <c r="B67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+      <c r="A68">
         <v>85</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C68" s="1" t="s">
+      <c r="B68" t="s">
+        <v>64</v>
+      </c>
+      <c r="C68" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+      <c r="A69">
         <v>86</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C69" s="1" t="s">
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+      <c r="A70">
         <v>87</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C70" s="1" t="s">
+      <c r="B70" t="s">
+        <v>64</v>
+      </c>
+      <c r="C70" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+      <c r="A71">
         <v>88</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C71" s="1" t="s">
+      <c r="B71" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+      <c r="A72">
         <v>89</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C72" s="1" t="s">
+      <c r="B72" t="s">
+        <v>64</v>
+      </c>
+      <c r="C72" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+      <c r="A73">
         <v>90</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C73" s="1" t="s">
+      <c r="B73" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+      <c r="A74">
         <v>91</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C74" s="1" t="s">
+      <c r="B74" t="s">
+        <v>64</v>
+      </c>
+      <c r="C74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+      <c r="A75">
         <v>92</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C75" s="1" t="s">
+      <c r="B75" t="s">
+        <v>64</v>
+      </c>
+      <c r="C75" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+      <c r="A76">
         <v>93</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C76" s="1" t="s">
+      <c r="B76" t="s">
+        <v>64</v>
+      </c>
+      <c r="C76" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+      <c r="A77">
         <v>94</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C77" s="1" t="s">
+      <c r="B77" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+      <c r="A78">
         <v>95</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C78" s="1" t="s">
+      <c r="B78" t="s">
+        <v>64</v>
+      </c>
+      <c r="C78" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+      <c r="A79">
         <v>96</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C79" s="1" t="s">
+      <c r="B79" t="s">
+        <v>64</v>
+      </c>
+      <c r="C79" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+      <c r="A80">
         <v>97</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C80" s="1" t="s">
+      <c r="B80" t="s">
+        <v>64</v>
+      </c>
+      <c r="C80" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+      <c r="A81">
         <v>98</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C81" s="1" t="s">
+      <c r="B81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="A82">
         <v>99</v>
       </c>
-      <c r="B82" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C82" s="1" t="s">
+      <c r="B82" t="s">
+        <v>64</v>
+      </c>
+      <c r="C82" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+      <c r="A83">
         <v>100</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C83" s="1" t="s">
+      <c r="B83" t="s">
+        <v>64</v>
+      </c>
+      <c r="C83" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+      <c r="A84">
         <v>101</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="B84" t="s">
+        <v>64</v>
+      </c>
+      <c r="C84" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+      <c r="A85">
         <v>102</v>
       </c>
-      <c r="B85" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C85" s="1" t="s">
+      <c r="B85" t="s">
+        <v>64</v>
+      </c>
+      <c r="C85" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+      <c r="A86">
         <v>103</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C86" s="1" t="s">
+      <c r="B86" t="s">
+        <v>64</v>
+      </c>
+      <c r="C86" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+      <c r="A87">
         <v>104</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C87" s="1" t="s">
+      <c r="B87" t="s">
+        <v>64</v>
+      </c>
+      <c r="C87" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+      <c r="A88">
         <v>105</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C88" s="1" t="s">
+      <c r="B88" t="s">
+        <v>64</v>
+      </c>
+      <c r="C88" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+      <c r="A89">
         <v>106</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C89" s="1" t="s">
+      <c r="B89" t="s">
+        <v>64</v>
+      </c>
+      <c r="C89" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+      <c r="A90">
         <v>107</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C90" s="1" t="s">
+      <c r="B90" t="s">
+        <v>64</v>
+      </c>
+      <c r="C90" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+      <c r="A91">
         <v>108</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C91" s="1" t="s">
+      <c r="B91" t="s">
+        <v>64</v>
+      </c>
+      <c r="C91" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+      <c r="A92">
         <v>109</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C92" s="1" t="s">
+      <c r="B92" t="s">
+        <v>64</v>
+      </c>
+      <c r="C92" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+      <c r="A93">
         <v>110</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C93" s="1" t="s">
+      <c r="B93" t="s">
+        <v>64</v>
+      </c>
+      <c r="C93" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+      <c r="A94">
         <v>111</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C94" s="1" t="s">
+      <c r="B94" t="s">
+        <v>64</v>
+      </c>
+      <c r="C94" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+      <c r="A95">
         <v>112</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C95" s="1" t="s">
+      <c r="B95" t="s">
+        <v>64</v>
+      </c>
+      <c r="C95" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+      <c r="A96">
         <v>113</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C96" s="1" t="s">
+      <c r="B96" t="s">
+        <v>64</v>
+      </c>
+      <c r="C96" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+      <c r="A97">
         <v>114</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>25</v>
+      <c r="B97" t="s">
+        <v>64</v>
+      </c>
+      <c r="C97" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>115</v>
+      </c>
+      <c r="B98" s="1">
+        <v>0</v>
+      </c>
+      <c r="C98" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>